<commit_message>
posted midterm 2 gradelines
</commit_message>
<xml_diff>
--- a/213_F24/gradelines.xlsx
+++ b/213_F24/gradelines.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="E2" s="3">
         <f>100*(SUM(F5:F14)/COUNT(F5:F14)*0.15 + SUM(F18:F27)/COUNT(F18:F27)*0.1 + SUM(F31:F33)*0.15 + F34*0.3)</f>
-        <v>24</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="3">
@@ -623,7 +623,7 @@
         <v>20.0</v>
       </c>
       <c r="F9" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -639,7 +639,7 @@
         <v>20.0</v>
       </c>
       <c r="F10" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -655,7 +655,7 @@
         <v>20.0</v>
       </c>
       <c r="F11" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>20</v>
@@ -702,21 +702,23 @@
       </c>
       <c r="I12" s="11">
         <f>0.93*E15</f>
-        <v>74.4</v>
+        <v>130.2</v>
       </c>
       <c r="J12" s="11">
         <f>0.93*E28</f>
-        <v>33.48</v>
+        <v>55.8</v>
       </c>
       <c r="K12" s="11">
         <v>79.0</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="11">
+        <v>72.0</v>
+      </c>
       <c r="M12" s="7"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11">
         <f>IF(E15=0, 0, I12/E15)*I25 + IF(E28=0, 0, J12/E28)*J25 + IF(E31=0, 0, K12/E31)*K25 + IF(E32=0, 0, L12/E32)*L25 + IF(E33=0, 0, M12/E33)*M25 + IF(E34=0, 0, N12/E34)*N25</f>
-        <v>92.95588235</v>
+        <v>89.86764706</v>
       </c>
     </row>
     <row r="13">
@@ -739,21 +741,23 @@
       </c>
       <c r="I13" s="11">
         <f>0.9*E15</f>
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="J13" s="12">
         <f>0.9*E28</f>
-        <v>32.4</v>
+        <v>54</v>
       </c>
       <c r="K13" s="11">
         <v>76.5</v>
       </c>
-      <c r="L13" s="11"/>
+      <c r="L13" s="11">
+        <v>67.0</v>
+      </c>
       <c r="M13" s="7"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11">
         <f>IF(E15=0, 0, I13/E15)*I25 + IF(E28=0, 0, J13/E28)*J25 + IF(E31=0, 0, K13/E31)*K25 + IF(E32=0, 0, L13/E32)*L25 + IF(E33=0, 0, M13/E33)*M25 + IF(E34=0, 0, N13/E34)*N25</f>
-        <v>90</v>
+        <v>85.80882353</v>
       </c>
     </row>
     <row r="14">
@@ -776,21 +780,23 @@
       </c>
       <c r="I14" s="11">
         <f>0.87*E15</f>
-        <v>69.6</v>
+        <v>121.8</v>
       </c>
       <c r="J14" s="12">
         <f>0.87*E28</f>
-        <v>31.32</v>
+        <v>52.2</v>
       </c>
       <c r="K14" s="11">
         <v>73.5</v>
       </c>
-      <c r="L14" s="11"/>
+      <c r="L14" s="11">
+        <v>62.0</v>
+      </c>
       <c r="M14" s="7"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11">
         <f>IF(E15=0, 0, I14/E15)*I25 + IF(E28=0, 0, J14/E28)*J25 + IF(E31=0, 0, K14/E31)*K25 + IF(E32=0, 0, L14/E32)*L25 + IF(E33=0, 0, M14/E33)*M25 + IF(E34=0, 0, N14/E34)*N25</f>
-        <v>86.60294118</v>
+        <v>81.52941176</v>
       </c>
     </row>
     <row r="15">
@@ -806,7 +812,7 @@
       </c>
       <c r="E15" s="7">
         <f>20*MIN(SUM(F5:F14),COUNT(F5:F14)-1)</f>
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="F15" s="7"/>
       <c r="H15" s="7" t="s">
@@ -814,21 +820,23 @@
       </c>
       <c r="I15" s="11">
         <f>0.83*E15</f>
-        <v>66.4</v>
+        <v>116.2</v>
       </c>
       <c r="J15" s="12">
         <f>0.83*E28</f>
-        <v>29.88</v>
+        <v>49.8</v>
       </c>
       <c r="K15" s="11">
         <v>70.5</v>
       </c>
-      <c r="L15" s="11"/>
+      <c r="L15" s="11">
+        <v>57.0</v>
+      </c>
       <c r="M15" s="7"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11">
         <f>IF(E15=0, 0, I15/E15)*I25 + IF(E28=0, 0, J15/E28)*J25 + IF(E31=0, 0, K15/E31)*K25 + IF(E32=0, 0, L15/E32)*L25 + IF(E33=0, 0, M15/E33)*M25 + IF(E34=0, 0, N15/E34)*N25</f>
-        <v>82.95588235</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -842,21 +850,23 @@
       </c>
       <c r="I16" s="11">
         <f>0.8*E15</f>
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="J16" s="12">
         <f>0.8*E28</f>
-        <v>28.8</v>
+        <v>48</v>
       </c>
       <c r="K16" s="11">
         <v>68.0</v>
       </c>
-      <c r="L16" s="11"/>
+      <c r="L16" s="11">
+        <v>52.0</v>
+      </c>
       <c r="M16" s="7"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11">
         <f>IF(E15=0, 0, I16/E15)*I25 + IF(E28=0, 0, J16/E28)*J25 + IF(E31=0, 0, K16/E31)*K25 + IF(E32=0, 0, L16/E32)*L25 + IF(E33=0, 0, M16/E33)*M25 + IF(E34=0, 0, N16/E34)*N25</f>
-        <v>80</v>
+        <v>72.94117647</v>
       </c>
     </row>
     <row r="17">
@@ -880,21 +890,23 @@
       </c>
       <c r="I17" s="12">
         <f>0.77*E15</f>
-        <v>61.6</v>
+        <v>107.8</v>
       </c>
       <c r="J17" s="12">
         <f>0.77*E28</f>
-        <v>27.72</v>
+        <v>46.2</v>
       </c>
       <c r="K17" s="11">
         <v>65.0</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="11">
+        <v>46.0</v>
+      </c>
       <c r="M17" s="7"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11">
         <f>IF(E15=0, 0, I17/E15)*I25 + IF(E28=0, 0, J17/E28)*J25 + IF(E31=0, 0, K17/E31)*K25 + IF(E32=0, 0, L17/E32)*L25 + IF(E33=0, 0, M17/E33)*M25 + IF(E34=0, 0, N17/E34)*N25</f>
-        <v>76.60294118</v>
+        <v>68.22058824</v>
       </c>
     </row>
     <row r="18">
@@ -917,21 +929,23 @@
       </c>
       <c r="I18" s="12">
         <f>0.73*E15</f>
-        <v>58.4</v>
+        <v>102.2</v>
       </c>
       <c r="J18" s="12">
         <f>0.73*E28</f>
-        <v>26.28</v>
+        <v>43.8</v>
       </c>
       <c r="K18" s="11">
         <v>61.0</v>
       </c>
-      <c r="L18" s="11"/>
+      <c r="L18" s="11">
+        <v>40.0</v>
+      </c>
       <c r="M18" s="7"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11">
         <f>IF(E15=0, 0, I18/E15)*I25 + IF(E28=0, 0, J18/E28)*J25 + IF(E31=0, 0, K18/E31)*K25 + IF(E32=0, 0, L18/E32)*L25 + IF(E33=0, 0, M18/E33)*M25 + IF(E34=0, 0, N18/E34)*N25</f>
-        <v>72.07352941</v>
+        <v>62.80882353</v>
       </c>
     </row>
     <row r="19">
@@ -954,21 +968,23 @@
       </c>
       <c r="I19" s="11">
         <f>0.7*E15</f>
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="J19" s="12">
         <f>0.7*E28</f>
-        <v>25.2</v>
+        <v>42</v>
       </c>
       <c r="K19" s="11">
         <v>57.0</v>
       </c>
-      <c r="L19" s="11"/>
+      <c r="L19" s="11">
+        <v>34.0</v>
+      </c>
       <c r="M19" s="7"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11">
         <f>IF(E15=0, 0, I19/E15)*I25 + IF(E28=0, 0, J19/E28)*J25 + IF(E31=0, 0, K19/E31)*K25 + IF(E32=0, 0, L19/E32)*L25 + IF(E33=0, 0, M19/E33)*M25 + IF(E34=0, 0, N19/E34)*N25</f>
-        <v>67.79411765</v>
+        <v>57.64705882</v>
       </c>
     </row>
     <row r="20">
@@ -991,21 +1007,23 @@
       </c>
       <c r="I20" s="11">
         <f>0.67*E15</f>
-        <v>53.6</v>
+        <v>93.8</v>
       </c>
       <c r="J20" s="12">
         <f>0.67*E28</f>
-        <v>24.12</v>
+        <v>40.2</v>
       </c>
       <c r="K20" s="11">
         <v>52.0</v>
       </c>
-      <c r="L20" s="11"/>
+      <c r="L20" s="11">
+        <v>29.0</v>
+      </c>
       <c r="M20" s="7"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11">
         <f>IF(E15=0, 0, I20/E15)*I25 + IF(E28=0, 0, J20/E28)*J25 + IF(E31=0, 0, K20/E31)*K25 + IF(E32=0, 0, L20/E32)*L25 + IF(E33=0, 0, M20/E33)*M25 + IF(E34=0, 0, N20/E34)*N25</f>
-        <v>62.63235294</v>
+        <v>52.48529412</v>
       </c>
     </row>
     <row r="21">
@@ -1021,28 +1039,30 @@
         <v>12.0</v>
       </c>
       <c r="F21" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I21" s="11">
         <f>0.63*E15</f>
-        <v>50.4</v>
+        <v>88.2</v>
       </c>
       <c r="J21" s="12">
         <f>0.63*E28</f>
-        <v>22.68</v>
+        <v>37.8</v>
       </c>
       <c r="K21" s="11">
         <v>47.0</v>
       </c>
-      <c r="L21" s="11"/>
+      <c r="L21" s="11">
+        <v>25.0</v>
+      </c>
       <c r="M21" s="7"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11">
         <f>IF(E15=0, 0, I21/E15)*I25 + IF(E28=0, 0, J21/E28)*J25 + IF(E31=0, 0, K21/E31)*K25 + IF(E32=0, 0, L21/E32)*L25 + IF(E33=0, 0, M21/E33)*M25 + IF(E34=0, 0, N21/E34)*N25</f>
-        <v>57.22058824</v>
+        <v>47.51470588</v>
       </c>
     </row>
     <row r="22">
@@ -1058,28 +1078,30 @@
         <v>12.0</v>
       </c>
       <c r="F22" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I22" s="11">
         <f>0.6*E15</f>
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="J22" s="12">
         <f>0.6*E28</f>
-        <v>21.6</v>
+        <v>36</v>
       </c>
       <c r="K22" s="11">
         <v>42.0</v>
       </c>
-      <c r="L22" s="11"/>
+      <c r="L22" s="11">
+        <v>20.0</v>
+      </c>
       <c r="M22" s="7"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11">
         <f>IF(E15=0, 0, I22/E15)*I25 + IF(E28=0, 0, J22/E28)*J25 + IF(E31=0, 0, K22/E31)*K25 + IF(E32=0, 0, L22/E32)*L25 + IF(E33=0, 0, M22/E33)*M25 + IF(E34=0, 0, N22/E34)*N25</f>
-        <v>52.05882353</v>
+        <v>42.35294118</v>
       </c>
     </row>
     <row r="23">
@@ -1111,7 +1133,9 @@
       <c r="K23" s="11">
         <v>0.0</v>
       </c>
-      <c r="L23" s="11"/>
+      <c r="L23" s="11">
+        <v>0.0</v>
+      </c>
       <c r="M23" s="7"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11">
@@ -1192,11 +1216,11 @@
       </c>
       <c r="K25" s="11">
         <f>75*F31/(F31+F32+F33+2*F34)</f>
-        <v>75</v>
+        <v>37.5</v>
       </c>
       <c r="L25" s="11">
         <f>75*F32/(F31+F32+F33+2*F34)</f>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="M25" s="11">
         <f>75*F33/(F31+F32+F33+2*F34)</f>
@@ -1264,7 +1288,7 @@
       </c>
       <c r="E28" s="7">
         <f>12*MIN(SUM(F18:F27),COUNT(F18:F27)-2)</f>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F28" s="7"/>
       <c r="I28" s="6"/>
@@ -1322,9 +1346,11 @@
       <c r="D32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="7">
+        <v>85.0</v>
+      </c>
       <c r="F32" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">

</xml_diff>

<commit_message>
updated gradelines, posted f-exam solutions
</commit_message>
<xml_diff>
--- a/213_F24/gradelines.xlsx
+++ b/213_F24/gradelines.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="E2" s="4">
         <f>100*(SUM(F5:F15)/COUNT(F5:F15)*0.15 + SUM(F19:F27)/COUNT(F19:F27)*0.1 + SUM(F31:F33)*0.15 + F34*0.3)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -717,10 +717,12 @@
       <c r="M12" s="8">
         <v>72.5</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="12">
+        <v>128.0</v>
+      </c>
       <c r="O12" s="12">
         <f>IF(E16=0, 0, I12/E16)*I25 + IF(E28=0, 0, J12/E28)*J25 + IF(E31=0, 0, K12/E31)*K25 + IF(E32=0, 0, L12/E32)*L25 + IF(E33=0, 0, M12/E33)*M25 + IF(E34=0, 0, N12/E34)*N25</f>
-        <v>90.89894419</v>
+        <v>91.07340907</v>
       </c>
     </row>
     <row r="13">
@@ -758,10 +760,12 @@
       <c r="M13" s="8">
         <v>70.0</v>
       </c>
-      <c r="N13" s="12"/>
+      <c r="N13" s="12">
+        <v>120.0</v>
+      </c>
       <c r="O13" s="12">
         <f>IF(E16=0, 0, I13/E16)*I25 + IF(E28=0, 0, J13/E28)*J25 + IF(E31=0, 0, K13/E31)*K25 + IF(E32=0, 0, L13/E32)*L25 + IF(E33=0, 0, M13/E33)*M25 + IF(E34=0, 0, N13/E34)*N25</f>
-        <v>87.14177979</v>
+        <v>86.81698277</v>
       </c>
     </row>
     <row r="14">
@@ -799,10 +803,12 @@
       <c r="M14" s="8">
         <v>67.5</v>
       </c>
-      <c r="N14" s="12"/>
+      <c r="N14" s="12">
+        <v>112.0</v>
+      </c>
       <c r="O14" s="12">
         <f>IF(E16=0, 0, I14/E16)*I25 + IF(E28=0, 0, J14/E28)*J25 + IF(E31=0, 0, K14/E31)*K25 + IF(E32=0, 0, L14/E32)*L25 + IF(E33=0, 0, M14/E33)*M25 + IF(E34=0, 0, N14/E34)*N25</f>
-        <v>83.23755656</v>
+        <v>82.47232117</v>
       </c>
     </row>
     <row r="15">
@@ -840,10 +846,12 @@
       <c r="M15" s="8">
         <v>64.0</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="12">
+        <v>104.0</v>
+      </c>
       <c r="O15" s="12">
         <f>IF(E16=0, 0, I15/E16)*I25 + IF(E28=0, 0, J15/E28)*J25 + IF(E31=0, 0, K15/E31)*K25 + IF(E32=0, 0, L15/E32)*L25 + IF(E33=0, 0, M15/E33)*M25 + IF(E34=0, 0, N15/E34)*N25</f>
-        <v>78.76282051</v>
+        <v>77.68535188</v>
       </c>
     </row>
     <row r="16">
@@ -882,10 +890,12 @@
       <c r="M16" s="8">
         <v>61.0</v>
       </c>
-      <c r="N16" s="12"/>
+      <c r="N16" s="12">
+        <v>95.0</v>
+      </c>
       <c r="O16" s="12">
         <f>IF(E16=0, 0, I16/E16)*I25 + IF(E28=0, 0, J16/E28)*J25 + IF(E31=0, 0, K16/E31)*K25 + IF(E32=0, 0, L16/E32)*L25 + IF(E33=0, 0, M16/E33)*M25 + IF(E34=0, 0, N16/E34)*N25</f>
-        <v>74.8453997</v>
+        <v>73.12000578</v>
       </c>
     </row>
     <row r="17">
@@ -914,10 +924,12 @@
       <c r="M17" s="8">
         <v>57.0</v>
       </c>
-      <c r="N17" s="12"/>
+      <c r="N17" s="12">
+        <v>85.0</v>
+      </c>
       <c r="O17" s="12">
         <f>IF(E16=0, 0, I17/E16)*I25 + IF(E28=0, 0, J17/E28)*J25 + IF(E31=0, 0, K17/E31)*K25 + IF(E32=0, 0, L17/E32)*L25 + IF(E33=0, 0, M17/E33)*M25 + IF(E34=0, 0, N17/E34)*N25</f>
-        <v>70.16628959</v>
+        <v>67.88488014</v>
       </c>
     </row>
     <row r="18">
@@ -956,10 +968,12 @@
       <c r="M18" s="8">
         <v>53.0</v>
       </c>
-      <c r="N18" s="12"/>
+      <c r="N18" s="12">
+        <v>74.0</v>
+      </c>
       <c r="O18" s="12">
         <f>IF(E16=0, 0, I18/E16)*I25 + IF(E28=0, 0, J18/E28)*J25 + IF(E31=0, 0, K18/E31)*K25 + IF(E32=0, 0, L18/E32)*L25 + IF(E33=0, 0, M18/E33)*M25 + IF(E34=0, 0, N18/E34)*N25</f>
-        <v>64.94306184</v>
+        <v>62.01051796</v>
       </c>
     </row>
     <row r="19">
@@ -997,10 +1011,12 @@
       <c r="M19" s="8">
         <v>48.0</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="12">
+        <v>64.0</v>
+      </c>
       <c r="O19" s="12">
         <f>IF(E16=0, 0, I19/E16)*I25 + IF(E28=0, 0, J19/E28)*J25 + IF(E31=0, 0, K19/E31)*K25 + IF(E32=0, 0, L19/E32)*L25 + IF(E33=0, 0, M19/E33)*M25 + IF(E34=0, 0, N19/E34)*N25</f>
-        <v>59.64932127</v>
+        <v>56.40661404</v>
       </c>
     </row>
     <row r="20">
@@ -1038,10 +1054,12 @@
       <c r="M20" s="8">
         <v>43.0</v>
       </c>
-      <c r="N20" s="12"/>
+      <c r="N20" s="12">
+        <v>54.0</v>
+      </c>
       <c r="O20" s="12">
         <f>IF(E16=0, 0, I20/E16)*I25 + IF(E28=0, 0, J20/E28)*J25 + IF(E31=0, 0, K20/E31)*K25 + IF(E32=0, 0, L20/E32)*L25 + IF(E33=0, 0, M20/E33)*M25 + IF(E34=0, 0, N20/E34)*N25</f>
-        <v>54.35558069</v>
+        <v>50.80271012</v>
       </c>
     </row>
     <row r="21">
@@ -1079,10 +1097,12 @@
       <c r="M21" s="8">
         <v>38.0</v>
       </c>
-      <c r="N21" s="12"/>
+      <c r="N21" s="12">
+        <v>44.0</v>
+      </c>
       <c r="O21" s="12">
         <f>IF(E16=0, 0, I21/E16)*I25 + IF(E28=0, 0, J21/E28)*J25 + IF(E31=0, 0, K21/E31)*K25 + IF(E32=0, 0, L21/E32)*L25 + IF(E33=0, 0, M21/E33)*M25 + IF(E34=0, 0, N21/E34)*N25</f>
-        <v>49.10595777</v>
+        <v>45.12527679</v>
       </c>
     </row>
     <row r="22">
@@ -1120,10 +1140,12 @@
       <c r="M22" s="8">
         <v>30.0</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="12">
+        <v>34.0</v>
+      </c>
       <c r="O22" s="12">
         <f>IF(E16=0, 0, I22/E16)*I25 + IF(E28=0, 0, J22/E28)*J25 + IF(E31=0, 0, K22/E31)*K25 + IF(E32=0, 0, L22/E32)*L25 + IF(E33=0, 0, M22/E33)*M25 + IF(E34=0, 0, N22/E34)*N25</f>
-        <v>42.85067873</v>
+        <v>38.94444979</v>
       </c>
     </row>
     <row r="23">
@@ -1161,7 +1183,9 @@
       <c r="M23" s="8">
         <v>0.0</v>
       </c>
-      <c r="N23" s="12"/>
+      <c r="N23" s="12">
+        <v>0.0</v>
+      </c>
       <c r="O23" s="12">
         <f>IF(E16=0, 0, I23/E16)*I25 + IF(E28=0, 0, J23/E28)*J25 + IF(E31=0, 0, K23/E31)*K25 + IF(E32=0, 0, L23/E32)*L25 + IF(E33=0, 0, M23/E33)*M25 + IF(E34=0, 0, N23/E34)*N25</f>
         <v>0</v>
@@ -1240,19 +1264,19 @@
       </c>
       <c r="K25" s="12">
         <f>75*F31/(F31+F32+F33+2*F34)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L25" s="12">
         <f>75*F32/(F31+F32+F33+2*F34)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="M25" s="12">
         <f>75*F33/(F31+F32+F33+2*F34)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="N25" s="12">
         <f>75*2*F34/(F31+F32+F33+2*F34)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O25" s="12">
         <f>SUM(I25:N25)</f>
@@ -1396,9 +1420,11 @@
       <c r="D34" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <v>141.0</v>
+      </c>
       <c r="F34" s="8">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="35">

</xml_diff>